<commit_message>
Updated names in gcmTable
</commit_message>
<xml_diff>
--- a/gcmTableData/gcmTable.xlsx
+++ b/gcmTableData/gcmTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/dmontgo2_nrel_gov/Documents/Projects/SAF-VTO/GCMPython/GroupContributionMethod/Solver_Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/dmontgo2_nrel_gov/Documents/Projects/SAF-VTO/GCM/GCM-Python/gcmTableData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{392AFA9E-7F5D-204F-9F8E-6CF234A12925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A272CADE-81B5-7A43-92D7-2D31EF320C34}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{F3978898-38A0-2147-92AF-74363453F93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32240" yWindow="500" windowWidth="27240" windowHeight="16440" xr2:uid="{B08CE4D9-0342-4148-B2BE-2317BF795217}"/>
+    <workbookView xWindow="21420" yWindow="1220" windowWidth="34560" windowHeight="22340" xr2:uid="{B08CE4D9-0342-4148-B2BE-2317BF795217}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,67 +407,67 @@
     <t>CHm(NH2)—COOH*</t>
   </si>
   <si>
-    <t>tfp1k</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
-    <t>tb1k</t>
-  </si>
-  <si>
-    <t>tc1k</t>
-  </si>
-  <si>
-    <t>pc1k</t>
-  </si>
-  <si>
     <t>bar^(-1/2)</t>
   </si>
   <si>
-    <t>vc1k</t>
-  </si>
-  <si>
     <t>m^3/kmol</t>
   </si>
   <si>
-    <t>w1k</t>
-  </si>
-  <si>
-    <t>hf1k</t>
-  </si>
-  <si>
     <t>kJ/mol</t>
   </si>
   <si>
-    <t>gf1k</t>
-  </si>
-  <si>
-    <t>hv1k</t>
-  </si>
-  <si>
     <t>KJ/mol</t>
   </si>
   <si>
-    <t>vliq1k</t>
-  </si>
-  <si>
-    <t>CpA1k</t>
-  </si>
-  <si>
     <t>J/mol/K</t>
   </si>
   <si>
-    <t>CpB1k</t>
-  </si>
-  <si>
-    <t>CpC1k</t>
-  </si>
-  <si>
     <t>MW</t>
   </si>
   <si>
     <t>g/mol</t>
+  </si>
+  <si>
+    <t>tck</t>
+  </si>
+  <si>
+    <t>pck</t>
+  </si>
+  <si>
+    <t>vck</t>
+  </si>
+  <si>
+    <t>tbk</t>
+  </si>
+  <si>
+    <t>tmk</t>
+  </si>
+  <si>
+    <t>hfk</t>
+  </si>
+  <si>
+    <t>gfk</t>
+  </si>
+  <si>
+    <t>hvk</t>
+  </si>
+  <si>
+    <t>wk</t>
+  </si>
+  <si>
+    <t>vmk</t>
+  </si>
+  <si>
+    <t>CpAk</t>
+  </si>
+  <si>
+    <t>CpBk</t>
+  </si>
+  <si>
+    <t>CpCk</t>
   </si>
 </sst>
 </file>
@@ -896,8 +896,8 @@
   <dimension ref="A1:DS15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D25" sqref="D25"/>
+      <pane xSplit="1" topLeftCell="CA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CE21" sqref="CE21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1275,10 +1275,10 @@
     </row>
     <row r="2" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C2" s="5">
         <v>1.6780999999999999</v>
@@ -1646,10 +1646,10 @@
     </row>
     <row r="3" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C3" s="5">
         <v>1.9900000000000001E-2</v>
@@ -2017,10 +2017,10 @@
     </row>
     <row r="4" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C4" s="5">
         <v>7.4999999999999997E-2</v>
@@ -2388,10 +2388,10 @@
     </row>
     <row r="5" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="7">
         <v>0.88939999999999997</v>
@@ -2759,10 +2759,10 @@
     </row>
     <row r="6" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="C6" s="4">
         <v>0.46400000000000002</v>
@@ -3130,10 +3130,10 @@
     </row>
     <row r="7" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C7" s="5">
         <v>-45.947000000000003</v>
@@ -3501,10 +3501,10 @@
     </row>
     <row r="8" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C8" s="5">
         <v>-8.0299999999999994</v>
@@ -3872,10 +3872,10 @@
     </row>
     <row r="9" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C9" s="5">
         <v>4.1159999999999997</v>
@@ -4243,7 +4243,7 @@
     </row>
     <row r="10" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -4614,10 +4614,10 @@
     </row>
     <row r="11" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C11" s="5">
         <v>2.6100000000000002E-2</v>
@@ -4985,10 +4985,10 @@
     </row>
     <row r="12" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C12" s="5">
         <v>35.115200000000002</v>
@@ -5356,10 +5356,10 @@
     </row>
     <row r="13" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C13" s="5">
         <v>39.592300000000002</v>
@@ -5727,10 +5727,10 @@
     </row>
     <row r="14" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C14" s="5">
         <v>-9.9231999999999996</v>
@@ -6098,10 +6098,10 @@
     </row>
     <row r="15" spans="1:123" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C15" s="5">
         <v>15</v>
@@ -6470,4 +6470,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{95965d95-ecc0-4720-b759-1f33c42ed7da}" enabled="1" method="Standard" siteId="{a0f29d7e-28cd-4f54-8442-7885aee7c080}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>